<commit_message>
Default timezone fix in tests.
</commit_message>
<xml_diff>
--- a/spec/fixtures/spreadsheet_parser/game.xlsx
+++ b/spec/fixtures/spreadsheet_parser/game.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" mc:Ignorable="v2">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
   </authors>
@@ -34,31 +34,11 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">В ячейках столбца A может быть любой текст. Читаются только данные из столбца B.</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>-654</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>10</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
     <comment ref="A3" authorId="0">
       <text>
@@ -67,38 +47,18 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Формат времени: YYYY-MM-DD HH:MM</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>-654</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>1</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" mc:Ignorable="v2">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
   </authors>
@@ -110,31 +70,11 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Все поля обязательны для заполнения</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>-347</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>1</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
     <comment ref="A6" authorId="0">
       <text>
@@ -143,38 +83,18 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Чтение кодов уровня начинается с 6 строки.</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>12</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>-347</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>11</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" mc:Ignorable="v2">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
   </authors>
@@ -186,31 +106,11 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Все поля обязательны для заполнения</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>-558</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>1</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
     <comment ref="A6" authorId="0">
       <text>
@@ -219,38 +119,18 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Чтение кодов уровня начинается с 6 строки.</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>12</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>-558</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>11</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t xml:space="preserve">Название</t>
   </si>
@@ -265,6 +145,9 @@
   </si>
   <si>
     <t xml:space="preserve">Время старта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-07-01 00:00:00 UTC+3</t>
   </si>
   <si>
     <t xml:space="preserve">Уровень 1</t>
@@ -316,6 +199,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -337,6 +221,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -390,7 +275,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -417,15 +302,15 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="106.428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="105.295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,8 +333,8 @@
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>44013</v>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -477,9 +362,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.9234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="64.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="64.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,20 +372,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>15</v>
@@ -508,15 +393,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>5</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -524,7 +413,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>1</v>
@@ -532,7 +421,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
@@ -540,7 +429,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>1</v>
@@ -548,7 +437,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>1</v>
@@ -557,7 +446,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CСтраница &amp;P</oddFooter>
@@ -573,15 +462,15 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.3673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,20 +478,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>17</v>
@@ -610,7 +499,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>3</v>
@@ -622,7 +511,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -630,7 +519,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>1</v>
@@ -638,7 +527,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
@@ -646,7 +535,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>1</v>
@@ -654,7 +543,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>1</v>
@@ -666,7 +555,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CСтраница &amp;P</oddFooter>

</xml_diff>

<commit_message>
TimeZone fix in tests.
</commit_message>
<xml_diff>
--- a/spec/fixtures/spreadsheet_parser/game.xlsx
+++ b/spec/fixtures/spreadsheet_parser/game.xlsx
@@ -147,7 +147,7 @@
     <t xml:space="preserve">Время старта</t>
   </si>
   <si>
-    <t xml:space="preserve">2020-07-01 00:00:00 UTC+3</t>
+    <t xml:space="preserve">2020-07-01 00:00:00 +0300</t>
   </si>
   <si>
     <t xml:space="preserve">Уровень 1</t>
@@ -308,9 +308,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="105.295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="104.076530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,9 +361,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="64.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="63.4438775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,9 +466,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.3367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.2551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Multiple codes in one sector support. Closes #2.
</commit_message>
<xml_diff>
--- a/spec/fixtures/spreadsheet_parser/game.xlsx
+++ b/spec/fixtures/spreadsheet_parser/game.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="1" state="visible" r:id="rId2"/>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t xml:space="preserve">Название</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t xml:space="preserve">http://telegra.ph/Some-link-55-55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code1.3</t>
   </si>
 </sst>
 </file>
@@ -302,14 +311,15 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="104.076530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="100.566326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,13 +366,14 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="63.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,43 +413,43 @@
       <c r="B5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -458,16 +469,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="88.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,43 +519,52 @@
       <c r="B5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving dates in UT to far future and some rubocop fixes
</commit_message>
<xml_diff>
--- a/spec/fixtures/spreadsheet_parser/game.xlsx
+++ b/spec/fixtures/spreadsheet_parser/game.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -60,7 +60,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -96,7 +96,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -147,7 +147,7 @@
     <t xml:space="preserve">Время старта</t>
   </si>
   <si>
-    <t xml:space="preserve">2020-07-01 00:00:00 +0300</t>
+    <t xml:space="preserve">2050-07-01 00:00:00 +0300</t>
   </si>
   <si>
     <t xml:space="preserve">Уровень 1</t>
@@ -311,15 +311,15 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="100.566326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="100.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,7 +349,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CСтраница &amp;P</oddFooter>
@@ -365,15 +365,15 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="61.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +455,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CСтраница &amp;P</oddFooter>
@@ -471,15 +471,15 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="88.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="88.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,7 +573,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CСтраница &amp;P</oddFooter>

</xml_diff>